<commit_message>
implementacion de filtro para ofertas duplicadas
</commit_message>
<xml_diff>
--- a/data/cleaned_offers.xlsx
+++ b/data/cleaned_offers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>e82bf3b8-6038-40be-9c25-412854cd7995</t>
+          <t>4327226302</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3dcdb372-ee8b-48de-8b81-19b19ef6bc2e</t>
+          <t>4327106573</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,7 +524,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>b6a0e058-0670-4d04-943a-ce04111f7338</t>
+          <t>4343521499</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -552,7 +552,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>fddfe227-1c37-49ba-8a8d-39dc98059aa2</t>
+          <t>4343532281</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>276d2b56-49b1-48f3-86c3-a2ab4b2eb57d</t>
+          <t>4338300150</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -609,7 +609,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>a5e0eca6-686b-4d51-9e6b-eb93cb659b90</t>
+          <t>4338260266</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a3631e49-a986-4530-96e5-f5dcce805416</t>
+          <t>4291659031</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -660,6 +660,63 @@
       <c r="F8" t="inlineStr">
         <is>
           <t>EPAM is a leading gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>4343326779</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4343326779/</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-12-13T15:35:28+00:00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>«Computer vision»: Remote AI Engineer - HireLATAM y más</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">En Baufest, nuestra </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>4338290130</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/4338290130/</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-12-13T15:35:28+00:00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>«Computer vision»: Remote AI Engineer - HireLATAM y más</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Join Our Team
+Oowli</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mejora de get_last_offers para hacerla mas capaz frente a ofertas de computrabajo
</commit_message>
<xml_diff>
--- a/data/cleaned_offers.xlsx
+++ b/data/cleaned_offers.xlsx
@@ -486,7 +486,9 @@
           <t>«Computer vision»: Sr. AI Engineer - Apptegy</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Who We Are
@@ -541,7 +543,9 @@
           <t>«tensorflow»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Job Title: Junior AI Engineer
@@ -580,7 +584,9 @@
           <t>«tensorflow»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>Work at DaCodes!
@@ -641,7 +647,9 @@
           <t>«tensorflow»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>We’re building AI-powered products, primarily leveraging off-the-shelf LLM APIs, while also partnering with our Applied Science teams to integrate custom models when needed. You’ll own end-to-end development of AI features—from prototyping to production—focused on reliability, accuracy, and scalable delivery.
@@ -697,7 +705,9 @@
           <t>«tensorflow»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>Work at DaCodes!
@@ -758,7 +768,9 @@
           <t>«tensorflow»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Job DescriptionJob Title: Mid-level AI Engineer
@@ -797,7 +809,9 @@
           <t>«tensorflow»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>Work at DaCodes!
@@ -858,7 +872,9 @@
           <t>«LLM»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>Job Title: Junior AI Engineer
@@ -897,7 +913,9 @@
           <t>«LLM»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>This is a remote position.
@@ -950,7 +968,9 @@
           <t>«LLM»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>6</v>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Job Title: Data Analyst (Remote)
@@ -985,7 +1005,9 @@
           <t>«LLM»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>Job DescriptionJob Title: Junior Data Science Associate Consultant
@@ -1019,7 +1041,9 @@
           <t>«LLM»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Job Title: Freelance Software Engineer - AI Projects (Remote)
@@ -1054,7 +1078,9 @@
           <t>«LLM»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>5</v>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>About Turing:Turing is one of the world’s fastest-growing AI companies, accelerating the advancement and deployment of powerful AI systems.
@@ -1090,7 +1116,9 @@
           <t>«desarrollador ia»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>3</v>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>¡Únete a Finandina BIC! Estamos buscando una mente estratégica y analítica con pasión:
@@ -1130,7 +1158,9 @@
           <t>«desarrollador ia»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>Job DescriptionJob Title: Junior Data Science Associate Consultant
@@ -1164,7 +1194,9 @@
           <t>«desarrollador ia»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>3</v>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>Founded in Palo Alto by Dr. Andrew Ng and Israel Niezen, Factored helps U.S. companies build and scale world-class AI, ML, and Data teams, powered by the top 1% of LATAM talent, with a defining purpose: To empower brilliant humans, unleash their potential, and amplify their impact in the world.
@@ -1206,7 +1238,9 @@
           <t>«desarrollador ia»: Junior AI Engineer (LATAM) - micro1 y más</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>6</v>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>Software Engineer — Spanish &amp; English Proficiency (Remote)Work Arrangement: RemoteEngagement Type: Independent ContractorHours: Flexible (5–40 hours per week)
@@ -1242,7 +1276,9 @@
           <t>«machine learning»: Junior Data Science Associate Consultant - LATAM - micro1 y más</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>Job DescriptionJob Title: Mid-level Data Science Associate Consultant
@@ -1277,7 +1313,9 @@
           <t>«Scikit-learn»: Forward Deployed Engineer - Andela</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>3</v>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>About AndelaAndela exists to connect brilliance and opportunity. Since 2014, we have been dedicated to breaking down global barriers and accelerating the future of work for both technologists and organizations around the world. For technologists, Andela offers competitive long-term career opportunities with leading organizations, access to a global community of professionals, and educational opportunities with leading technology providers.
@@ -1319,7 +1357,9 @@
           <t>«desarrollador ia»: Data Analyst (Remote) - Work Vista y más</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>Job Title: Data Analyst (Remote)
@@ -1354,7 +1394,9 @@
           <t>«desarrollador ia»: Data Analyst (Remote) - Work Vista y más</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>HireLatam is a premier recruitment agency that places top Latin American talent in independent contractor roles in US companies. With a proven track record and a commitment to excellence, we're your trusted partner in the pursuit of career success. Our extensive network, personalized approach, and supportive guidance ensure that you're in the best hands to find your next job opportunity. Job Title: Remote AI Engineer (100% Work From Home) Location: Remote from Latin America Position Type: Full-time  Salary: $4,000 USD/month  Schedule: Monday-Friday, business hours in one of the major US time zones  Job Overview:We're building a pipeline of talented AI Engineers to join our portfolio of clients. This role combines cutting-edge AI/ML integration with practical software engineering to deliver production-ready solutions that automate workflows and enhance user experiences. You'll work on diverse projects ranging from document processing pipelines, transforming legacy workflows to LLM-powered personalization systems. Please keep in mind that the description below may vary depending on the specific client and role.  Responsibilities:AI/ML Development &amp; IntegrationBuild and deploy AI-driven features using LLMs and external AI APIs (OpenAI, Anthropic, Bedrock, Mistral)Design and implement backend services integrating retrieval systems, embeddings, and vector databases (pgvector, Pinecone)Develop OCR and computer vision pipelines using YOLO, AWS Textract, and ComprehendOrchestrate AI model calls with proper context management, caching, and prompt engineeringBackend EngineeringCreate Python microservices using FastAPI for ML/AI workloadsImplement and maintain Java Spring Boot microservices for enterprise integrationsBuild robust REST APIs with comprehensive integration testingDevelop connectors and adapters for vendor systems and legacy platform integrationMLOps &amp; Production EngineeringProductionize ML models with containerization (Docker), versioning, and evaluation frameworksImplement batch and async processing for scalable AI servicesSet up monitoring, logging, and fallback strategies for production AI systemsPackage and deploy models using AWS services (Lambda, SageMaker, Bedrock, Step Functions)Product DevelopmentPrototype and validate AI-powered features through rapid experimentationEvolve successful experiments into scalable, production-grade systemsCollaborate with cross-functional teams to translate product goals into robust AI featuresBuild internal tools and dashboards for model evaluation and monitoring Qualifications, Skills and Key Competencies:Technical Skills3-5 years of software engineering experience with both Java (Spring/Hibernate) and PythonStrong experience with AI frameworks, particularly LangChain or LlamaIndexHands-on experience with LLMs and RAG patterns for retrieval-based systemsProficiency with ML workflows using NumPy, Pandas, scikit-learn, or TensorFlow/KerasExperience with both SQL databases (MySQL, PostgreSQL) and NoSQL (MongoDB)Strong AWS experience (Lambda, S3, SQS/SNS, KMS, Step Functions)Proficiency with Docker, Git, and CI/CD practicesExperience with message brokers, streaming systems, and microservice patternsAI/ML Specific ExperiencePractical experience with prompt engineering and LLM optimizationFamiliarity with vector databases and embedding systemsExperience with OCR pipelines and computer vision applicationsKnowledge of MLOps practices including MLflow, DVC, model versioningNice to HaveFrontend development skills (React/Vue) for building internal toolsExperience building conversational or agentic AI systemsExperience with distributed systems and cloud-native architecturesFamiliarity with evaluation frameworks and A/B testing for AI featuresSoft SkillsStrong product mindset with ability to balance performance, reliability, and costSelf-motivated and adaptable with eagerness to embrace new challengesExcellent problem-solving and analytical thinking abilitiesStrong communication skills in written English and SpanishAbility to work effectively in cross-functional teamsExample Projects You'll Work OnVendor &amp; AI Model Integration: Execute integration projects with external AI providers to automate internal operations and customer-facing processesAI-Driven Workflow Automation: Implement LLM-powered decision-making and document processing pipelines to streamline validation and screening workflowsPersonalization Systems: Build AI features that create personalized experiences for thousands of users across multiple regionsLegacy System Modernization: Develop adapters and middleware enabling AI-enhanced services to interoperate with existing systems during migrationWhat We OfferOpportunity to work on cutting-edge AI/ML technologies in production environmentsRemote-first work environment with flexible hoursCollaboration with talented engineers and product teamsDirect impact on products serving thousands of usersContinuous learning and professional development opportunities</t>
@@ -1382,7 +1424,9 @@
           <t>«desarrollador ia»: Data Analyst (Remote) - Work Vista y más</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>3</v>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>At BairesDev®, we've been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.
@@ -1422,7 +1466,9 @@
           <t>«desarrollador ia»: Data Analyst (Remote) - Work Vista y más</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>5</v>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>Job Title: Freelance Software Engineer - AI Projects (Remote)
@@ -1457,7 +1503,9 @@
           <t>«desarrollador ia»: Data Analyst (Remote) - Work Vista y más</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>3</v>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>At BairesDev®, we've been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.
@@ -1496,7 +1544,9 @@
           <t>«desarrollador ia»: Data Analyst (Remote) - Work Vista y más</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>3</v>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>Please submit your resume in English and indicate your level of English proficiency.
@@ -1529,7 +1579,9 @@
           <t>«pytorch»:  Remote AI Engineer - HireLATAM y más</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="n">
+        <v>3</v>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.
@@ -1567,7 +1619,9 @@
           <t>«pytorch»:  Remote AI Engineer - HireLATAM y más</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="n">
+        <v>3</v>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>At BairesDev®, we've been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.
@@ -1606,7 +1660,9 @@
           <t>«pytorch»:  Remote AI Engineer - HireLATAM y más</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="n">
+        <v>3</v>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>At BairesDev®, we've been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.

</xml_diff>